<commit_message>
have columns straight and all seems to be working pretty well
</commit_message>
<xml_diff>
--- a/uploads/ddos_test.xlsx
+++ b/uploads/ddos_test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Company Name</t>
   </si>
@@ -23,12 +23,6 @@
   </si>
   <si>
     <t>www.oakstreethealth.com</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>www.illinoisstate.edu</t>
   </si>
   <si>
     <t>Akamai Inc</t>
@@ -368,14 +362,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -383,8 +369,7 @@
     <hyperlink r:id="rId3" ref="B4"/>
     <hyperlink r:id="rId4" ref="B5"/>
     <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added clear filter button and fixed the spacing between filters
</commit_message>
<xml_diff>
--- a/uploads/ddos_test.xlsx
+++ b/uploads/ddos_test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Company Name</t>
   </si>
@@ -47,13 +47,19 @@
   </si>
   <si>
     <t>www.sourcebooks.com</t>
+  </si>
+  <si>
+    <t>Incap Co</t>
+  </si>
+  <si>
+    <t>www.thepacket.ninja</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -64,6 +70,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -84,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -92,6 +102,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -362,6 +375,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -369,7 +390,8 @@
     <hyperlink r:id="rId3" ref="B4"/>
     <hyperlink r:id="rId4" ref="B5"/>
     <hyperlink r:id="rId5" ref="B6"/>
+    <hyperlink r:id="rId6" ref="B7"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>